<commit_message>
Paketverlust: changed starting point of R0
</commit_message>
<xml_diff>
--- a/Theorie/GoBackN/Paketverlust.xlsx
+++ b/Theorie/GoBackN/Paketverlust.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josef\iCloudDrive\Documents\HTWG\Sem_5\Rechnernetze\Aufgaben\Theorie\GoBackN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josef\Documents\HTWG\Rechnernetze\Theorie\GoBackN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDFF46C-4E3C-43D6-BB27-369C4CCB1CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E81016-8250-42F3-83B4-8121D0BA6D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{69491014-9A9B-4CFF-8D82-84A350BFE43A}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="24675" windowHeight="10725" xr2:uid="{69491014-9A9B-4CFF-8D82-84A350BFE43A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -654,9 +654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2623F30B-D532-4166-93EC-EACEBFB4DBB0}">
   <dimension ref="A1:AE119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="58" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD119" sqref="AD119"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="2">
-        <f>A5+1+3</f>
+        <f>A5+3</f>
         <v>5</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -892,7 +892,8 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>0</v>
+        <f t="shared" ref="A4:A41" si="2">A3+1</f>
+        <v>1</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -919,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M3:M53" si="2">((1125 * L4)/6144) * 100</f>
+        <f t="shared" ref="M4" si="3">((1125 * L4)/6144) * 100</f>
         <v>0</v>
       </c>
       <c r="N4" s="3"/>
@@ -951,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <f t="shared" ref="AC4:AC67" si="3">((1125 * AB4)/(3 * 1024)) * 100</f>
+        <f t="shared" ref="AC4:AC67" si="4">((1125 * AB4)/(3 * 1024)) * 100</f>
         <v>0</v>
       </c>
       <c r="AD4" t="s">
@@ -963,8 +964,8 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A41" si="4">A4+1</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -1026,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD5" t="s">
@@ -1038,8 +1039,8 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1068,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="3">
-        <f>((1125 * L6)/6144) * 100</f>
+        <f t="shared" ref="M6:M37" si="9">((1125 * L6)/6144) * 100</f>
         <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -1087,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" ref="U6:U69" si="9">((1125 * T6)/(4 * 1024)) * 100</f>
+        <f t="shared" ref="U6:U69" si="10">((1125 * T6)/(4 * 1024)) * 100</f>
         <v>0</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1104,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="AC6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD6" t="s">
@@ -1116,8 +1117,8 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -1148,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="3">
-        <f>((1125 * L7)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N7" s="3"/>
@@ -1163,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V7" s="3" t="s">
@@ -1180,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="AC7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD7" t="s">
@@ -1192,8 +1193,8 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
@@ -1222,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="3">
-        <f>((1125 * L8)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N8" s="3"/>
@@ -1239,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V8" s="3" t="s">
@@ -1256,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="AC8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD8" t="s">
@@ -1268,8 +1269,8 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -1302,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="3">
-        <f>((1125 * L9)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -1323,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="U9" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V9" s="3" t="s">
@@ -1340,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="AC9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD9" t="s">
@@ -1352,8 +1353,8 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
@@ -1382,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <f>((1125 * L10)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N10" s="3"/>
@@ -1401,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="U10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V10" s="3" t="s">
@@ -1418,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="AC10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD10" t="s">
@@ -1430,8 +1431,8 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" si="4"/>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -1462,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <f>((1125 * L11)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N11" s="3"/>
@@ -1479,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="U11" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V11" s="3" t="s">
@@ -1502,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="AC11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD11" t="s">
@@ -1514,8 +1515,8 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
@@ -1546,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <f>((1125 * L12)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N12" s="3" t="s">
@@ -1565,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="U12" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1582,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="AC12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD12" t="s">
@@ -1594,8 +1595,8 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="4"/>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -1626,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3">
-        <f>((1125 * L13)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N13" s="3"/>
@@ -1641,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="U13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V13" s="3" t="s">
@@ -1658,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="AC13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD13" t="s">
@@ -1670,8 +1671,8 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -1700,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="3">
-        <f>((1125 * L14)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N14" s="3"/>
@@ -1717,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="U14" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V14" s="3" t="s">
@@ -1734,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD14" t="s">
@@ -1746,8 +1747,8 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="4"/>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
@@ -1780,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <f>((1125 * L15)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N15" s="3" t="s">
@@ -1801,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="U15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V15" s="3" t="s">
@@ -1818,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="AC15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD15" t="s">
@@ -1830,8 +1831,8 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -1860,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="3">
-        <f>((1125 * L16)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N16" s="3"/>
@@ -1879,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="U16" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V16" s="3" t="s">
@@ -1896,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="AC16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD16" t="s">
@@ -1909,7 +1910,7 @@
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>A16+1</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>12</v>
@@ -1940,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="3">
-        <f>((1125 * L17)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N17" s="3"/>
@@ -1957,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="U17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V17" s="3" t="s">
@@ -1974,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="AC17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD17" t="s">
@@ -1986,8 +1987,8 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -2018,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="3">
-        <f>((1125 * L18)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N18" s="3" t="s">
@@ -2039,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="U18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V18" s="3" t="s">
@@ -2056,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="AC18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD18" t="s">
@@ -2068,8 +2069,8 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
@@ -2100,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="3">
-        <f>((1125 * L19)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N19" s="3"/>
@@ -2117,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="U19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V19" s="3" t="s">
@@ -2140,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="AC19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD19" t="s">
@@ -2152,8 +2153,8 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
@@ -2182,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="3">
-        <f>((1125 * L20)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N20" s="3"/>
@@ -2201,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V20" s="3" t="s">
@@ -2221,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="AC20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD20" t="s">
@@ -2233,8 +2234,8 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>14</v>
@@ -2267,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="3">
-        <f>((1125 * L21)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N21" s="3" t="s">
@@ -2288,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="U21" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V21" s="3" t="s">
@@ -2305,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="AC21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD21" t="s">
@@ -2317,8 +2318,8 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -2347,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="3">
-        <f>((1125 * L22)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N22" s="3"/>
@@ -2366,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="U22" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V22" s="3" t="s">
@@ -2383,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="AC22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD22" t="s">
@@ -2395,8 +2396,8 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>15</v>
@@ -2427,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="3">
-        <f>((1125 * L23)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N23" s="3"/>
@@ -2444,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="U23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V23" s="3" t="s">
@@ -2461,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="AC23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD23" t="s">
@@ -2473,8 +2474,8 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
@@ -2505,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="3">
-        <f>((1125 * L24)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N24" s="3" t="s">
@@ -2526,7 +2527,7 @@
         <v>1</v>
       </c>
       <c r="U24" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V24" s="3" t="s">
@@ -2543,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="AC24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD24" t="s">
@@ -2555,8 +2556,8 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
-        <v>21</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>16</v>
@@ -2587,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="3">
-        <f>((1125 * L25)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N25" s="3"/>
@@ -2604,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="U25" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V25" s="3" t="s">
@@ -2621,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="AC25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD25" t="s">
@@ -2633,8 +2634,8 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -2663,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="3">
-        <f>((1125 * L26)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N26" s="3"/>
@@ -2682,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="U26" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V26" s="3" t="s">
@@ -2699,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="AC26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD26" t="s">
@@ -2711,8 +2712,8 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
@@ -2745,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="3">
-        <f>((1125 * L27)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N27" s="3" t="s">
@@ -2766,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="U27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V27" s="3" t="s">
@@ -2789,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="AC27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD27" t="s">
@@ -2801,8 +2802,8 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
@@ -2831,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="3">
-        <f>((1125 * L28)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N28" s="3"/>
@@ -2850,7 +2851,7 @@
         <v>2</v>
       </c>
       <c r="U28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V28" s="3" t="s">
@@ -2870,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="AC28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD28" t="s">
@@ -2882,8 +2883,8 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>18</v>
@@ -2914,7 +2915,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="3">
-        <f>((1125 * L29)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N29" s="3"/>
@@ -2931,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="U29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V29" s="3" t="s">
@@ -2951,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="AC29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD29" t="s">
@@ -2963,8 +2964,8 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -2995,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="3">
-        <f>((1125 * L30)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N30" s="3" t="s">
@@ -3016,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="U30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V30" s="3" t="s">
@@ -3033,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="AC30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD30" t="s">
@@ -3045,8 +3046,8 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>19</v>
@@ -3077,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="3">
-        <f>((1125 * L31)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N31" s="3"/>
@@ -3094,7 +3095,7 @@
         <v>1</v>
       </c>
       <c r="U31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V31" s="3" t="s">
@@ -3111,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="AC31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD31" t="s">
@@ -3123,8 +3124,8 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="4"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
@@ -3153,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="3">
-        <f>((1125 * L32)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N32" s="3"/>
@@ -3172,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="U32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.4658203125</v>
       </c>
       <c r="V32" s="3" t="s">
@@ -3189,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="AC32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD32" t="s">
@@ -3201,8 +3202,8 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="4"/>
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>20</v>
@@ -3235,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="3">
-        <f>((1125 * L33)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N33" s="3" t="s">
@@ -3256,7 +3257,7 @@
         <v>2</v>
       </c>
       <c r="U33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V33" s="3" t="s">
@@ -3273,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="AC33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD33" t="s">
@@ -3285,8 +3286,8 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -3315,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="3">
-        <f>((1125 * L34)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N34" s="3"/>
@@ -3334,7 +3335,7 @@
         <v>2</v>
       </c>
       <c r="U34" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V34" s="3" t="s">
@@ -3351,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="AC34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD34" t="s">
@@ -3363,8 +3364,8 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="4"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>21</v>
@@ -3395,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="3">
-        <f>((1125 * L35)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N35" s="3"/>
@@ -3412,7 +3413,7 @@
         <v>2</v>
       </c>
       <c r="U35" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V35" s="3" t="s">
@@ -3435,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="AC35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD35" t="s">
@@ -3447,8 +3448,8 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="4"/>
-        <v>32</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
@@ -3479,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <f>((1125 * L36)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N36" s="3" t="s">
@@ -3500,7 +3501,7 @@
         <v>2</v>
       </c>
       <c r="U36" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V36" s="3" t="s">
@@ -3520,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="AC36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD36" t="s">
@@ -3532,8 +3533,8 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="4"/>
-        <v>33</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>22</v>
@@ -3564,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <f>((1125 * L37)/6144) * 100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N37" s="3"/>
@@ -3581,7 +3582,7 @@
         <v>2</v>
       </c>
       <c r="U37" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V37" s="3" t="s">
@@ -3601,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="AC37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD37" t="s">
@@ -3613,8 +3614,8 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="4"/>
-        <v>34</v>
+        <f t="shared" si="2"/>
+        <v>35</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -3643,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="3">
-        <f>((1125 * L38)/6144) * 100</f>
+        <f t="shared" ref="M38:M69" si="11">((1125 * L38)/6144) * 100</f>
         <v>0</v>
       </c>
       <c r="N38" s="3"/>
@@ -3662,7 +3663,7 @@
         <v>2</v>
       </c>
       <c r="U38" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V38" s="3" t="s">
@@ -3682,7 +3683,7 @@
         <v>1</v>
       </c>
       <c r="AC38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD38" t="s">
@@ -3694,8 +3695,8 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <f t="shared" si="4"/>
-        <v>35</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>23</v>
@@ -3728,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="3">
-        <f>((1125 * L39)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N39" s="3" t="s">
@@ -3749,7 +3750,7 @@
         <v>2</v>
       </c>
       <c r="U39" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V39" s="3" t="s">
@@ -3766,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="AC39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD39" t="s">
@@ -3778,8 +3779,8 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <f t="shared" si="4"/>
-        <v>36</v>
+        <f t="shared" si="2"/>
+        <v>37</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
@@ -3808,7 +3809,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="3">
-        <f>((1125 * L40)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N40" s="3"/>
@@ -3827,7 +3828,7 @@
         <v>2</v>
       </c>
       <c r="U40" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V40" s="3" t="s">
@@ -3844,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="AC40" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD40" t="s">
@@ -3856,8 +3857,8 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <f t="shared" si="4"/>
-        <v>37</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>24</v>
@@ -3888,7 +3889,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="3">
-        <f>((1125 * L41)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N41" s="3"/>
@@ -3905,7 +3906,7 @@
         <v>2</v>
       </c>
       <c r="U41" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V41" s="3" t="s">
@@ -3922,7 +3923,7 @@
         <v>0</v>
       </c>
       <c r="AC41" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD41" t="s">
@@ -3965,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="3">
-        <f>((1125 * L42)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N42" s="3" t="s">
@@ -3986,7 +3987,7 @@
         <v>2</v>
       </c>
       <c r="U42" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V42" s="3" t="s">
@@ -4003,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="AC42" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD42" t="s">
@@ -4046,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="3">
-        <f>((1125 * L43)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N43" s="3"/>
@@ -4063,7 +4064,7 @@
         <v>2</v>
       </c>
       <c r="U43" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V43" s="3" t="s">
@@ -4086,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="AC43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD43" t="s">
@@ -4126,7 +4127,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="3">
-        <f>((1125 * L44)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N44" s="3"/>
@@ -4145,7 +4146,7 @@
         <v>2</v>
       </c>
       <c r="U44" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V44" s="3" t="s">
@@ -4165,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="AC44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD44" t="s">
@@ -4210,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="3">
-        <f>((1125 * L45)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N45" s="3" t="s">
@@ -4231,7 +4232,7 @@
         <v>3</v>
       </c>
       <c r="U45" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V45" s="3" t="s">
@@ -4251,7 +4252,7 @@
         <v>1</v>
       </c>
       <c r="AC45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD45" t="s">
@@ -4291,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="3">
-        <f>((1125 * L46)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N46" s="3"/>
@@ -4310,7 +4311,7 @@
         <v>3</v>
       </c>
       <c r="U46" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V46" s="3" t="s">
@@ -4330,7 +4331,7 @@
         <v>1</v>
       </c>
       <c r="AC46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD46" t="s">
@@ -4366,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="3">
-        <f>((1125 * L47)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N47" s="3"/>
@@ -4383,7 +4384,7 @@
         <v>3</v>
       </c>
       <c r="U47" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V47" s="3" t="s">
@@ -4403,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="AC47" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD47" t="s">
@@ -4426,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="3">
-        <f>((1125 * L48)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N48" s="3" t="s">
@@ -4447,7 +4448,7 @@
         <v>2</v>
       </c>
       <c r="U48" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V48" s="3" t="s">
@@ -4464,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="AC48" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD48" t="s">
@@ -4485,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="3">
-        <f>((1125 * L49)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N49" s="3"/>
@@ -4502,7 +4503,7 @@
         <v>2</v>
       </c>
       <c r="U49" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V49" s="3" t="s">
@@ -4519,7 +4520,7 @@
         <v>0</v>
       </c>
       <c r="AC49" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD49" t="s">
@@ -4540,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="3">
-        <f>((1125 * L50)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N50" s="3"/>
@@ -4559,7 +4560,7 @@
         <v>2</v>
       </c>
       <c r="U50" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V50" s="3" t="s">
@@ -4576,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="AC50" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD50" t="s">
@@ -4599,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="3">
-        <f>((1125 * L51)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N51" s="3" t="s">
@@ -4620,7 +4621,7 @@
         <v>3</v>
       </c>
       <c r="U51" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V51" s="3" t="s">
@@ -4643,7 +4644,7 @@
         <v>1</v>
       </c>
       <c r="AC51" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD51" t="s">
@@ -4664,7 +4665,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="3">
-        <f>((1125 * L52)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N52" s="3"/>
@@ -4683,7 +4684,7 @@
         <v>3</v>
       </c>
       <c r="U52" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V52" s="3" t="s">
@@ -4703,7 +4704,7 @@
         <v>1</v>
       </c>
       <c r="AC52" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD52" t="s">
@@ -4724,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="3">
-        <f>((1125 * L53)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N53" s="3"/>
@@ -4741,7 +4742,7 @@
         <v>3</v>
       </c>
       <c r="U53" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V53" s="3" t="s">
@@ -4761,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="AC53" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD53" t="s">
@@ -4781,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="3">
-        <f>((1125 * L54)/6144) * 100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N54" s="3" t="s">
@@ -4802,7 +4803,7 @@
         <v>3</v>
       </c>
       <c r="U54" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V54" s="3" t="s">
@@ -4822,7 +4823,7 @@
         <v>1</v>
       </c>
       <c r="AC54" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD54" t="s">
@@ -4845,7 +4846,7 @@
         <v>3</v>
       </c>
       <c r="U55" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V55" s="3" t="s">
@@ -4865,7 +4866,7 @@
         <v>1</v>
       </c>
       <c r="AC55" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD55" t="s">
@@ -4888,7 +4889,7 @@
         <v>3</v>
       </c>
       <c r="U56" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V56" s="3" t="s">
@@ -4908,7 +4909,7 @@
         <v>1</v>
       </c>
       <c r="AC56" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD56" t="s">
@@ -4933,7 +4934,7 @@
         <v>3</v>
       </c>
       <c r="U57" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V57" s="3" t="s">
@@ -4950,7 +4951,7 @@
         <v>0</v>
       </c>
       <c r="AC57" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD57" t="s">
@@ -4973,7 +4974,7 @@
         <v>3</v>
       </c>
       <c r="U58" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V58" s="3" t="s">
@@ -4990,7 +4991,7 @@
         <v>0</v>
       </c>
       <c r="AC58" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD58" t="s">
@@ -5013,7 +5014,7 @@
         <v>3</v>
       </c>
       <c r="U59" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V59" s="3" t="s">
@@ -5036,7 +5037,7 @@
         <v>1</v>
       </c>
       <c r="AC59" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD59" t="s">
@@ -5059,7 +5060,7 @@
         <v>3</v>
       </c>
       <c r="U60" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V60" s="3" t="s">
@@ -5079,7 +5080,7 @@
         <v>1</v>
       </c>
       <c r="AC60" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD60" t="s">
@@ -5102,7 +5103,7 @@
         <v>3</v>
       </c>
       <c r="U61" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V61" s="3" t="s">
@@ -5122,7 +5123,7 @@
         <v>1</v>
       </c>
       <c r="AC61" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD61" t="s">
@@ -5145,7 +5146,7 @@
         <v>3</v>
       </c>
       <c r="U62" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V62" s="3" t="s">
@@ -5165,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="AC62" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD62" t="s">
@@ -5190,7 +5191,7 @@
         <v>3</v>
       </c>
       <c r="U63" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V63" s="3" t="s">
@@ -5210,7 +5211,7 @@
         <v>1</v>
       </c>
       <c r="AC63" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD63" t="s">
@@ -5233,7 +5234,7 @@
         <v>3</v>
       </c>
       <c r="U64" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V64" s="3" t="s">
@@ -5253,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="AC64" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD64" t="s">
@@ -5276,7 +5277,7 @@
         <v>3</v>
       </c>
       <c r="U65" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V65" s="3" t="s">
@@ -5296,7 +5297,7 @@
         <v>1</v>
       </c>
       <c r="AC65" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD65" t="s">
@@ -5319,7 +5320,7 @@
         <v>2</v>
       </c>
       <c r="U66" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V66" s="3" t="s">
@@ -5336,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="AC66" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD66" t="s">
@@ -5359,7 +5360,7 @@
         <v>2</v>
       </c>
       <c r="U67" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V67" s="3" t="s">
@@ -5382,7 +5383,7 @@
         <v>1</v>
       </c>
       <c r="AC67" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.62109375</v>
       </c>
       <c r="AD67" t="s">
@@ -5405,7 +5406,7 @@
         <v>2</v>
       </c>
       <c r="U68" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.931640625</v>
       </c>
       <c r="V68" s="3" t="s">
@@ -5425,7 +5426,7 @@
         <v>1</v>
       </c>
       <c r="AC68" s="3">
-        <f t="shared" ref="AC68:AC115" si="10">((1125 * AB68)/(3 * 1024)) * 100</f>
+        <f t="shared" ref="AC68:AC115" si="12">((1125 * AB68)/(3 * 1024)) * 100</f>
         <v>36.62109375</v>
       </c>
       <c r="AD68" t="s">
@@ -5437,7 +5438,7 @@
     </row>
     <row r="69" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q69" s="2">
-        <f t="shared" ref="Q69:Q132" si="11">Q68+0.5</f>
+        <f t="shared" ref="Q69:Q105" si="13">Q68+0.5</f>
         <v>43</v>
       </c>
       <c r="R69" s="3" t="s">
@@ -5450,7 +5451,7 @@
         <v>3</v>
       </c>
       <c r="U69" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>82.3974609375</v>
       </c>
       <c r="V69" s="3" t="s">
@@ -5460,7 +5461,7 @@
         <v>3</v>
       </c>
       <c r="Y69" s="2">
-        <f t="shared" ref="Y69:Y115" si="12">Y68+0.5</f>
+        <f t="shared" ref="Y69:Y115" si="14">Y68+0.5</f>
         <v>57.5</v>
       </c>
       <c r="AA69" t="s">
@@ -5470,7 +5471,7 @@
         <v>1</v>
       </c>
       <c r="AC69" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD69" t="s">
@@ -5482,7 +5483,7 @@
     </row>
     <row r="70" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q70" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>43.5</v>
       </c>
       <c r="R70" s="3"/>
@@ -5493,7 +5494,7 @@
         <v>3</v>
       </c>
       <c r="U70" s="3">
-        <f t="shared" ref="U70:U133" si="13">((1125 * T70)/(4 * 1024)) * 100</f>
+        <f t="shared" ref="U70:U98" si="15">((1125 * T70)/(4 * 1024)) * 100</f>
         <v>82.3974609375</v>
       </c>
       <c r="V70" s="3" t="s">
@@ -5503,7 +5504,7 @@
         <v>2.5</v>
       </c>
       <c r="Y70" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>58</v>
       </c>
       <c r="AA70" t="s">
@@ -5513,7 +5514,7 @@
         <v>1</v>
       </c>
       <c r="AC70" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD70" t="s">
@@ -5525,7 +5526,7 @@
     </row>
     <row r="71" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q71" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44</v>
       </c>
       <c r="R71" s="3"/>
@@ -5536,7 +5537,7 @@
         <v>3</v>
       </c>
       <c r="U71" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V71" s="3" t="s">
@@ -5546,7 +5547,7 @@
         <v>2</v>
       </c>
       <c r="Y71" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>58.5</v>
       </c>
       <c r="AA71" t="s">
@@ -5556,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="AC71" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD71" t="s">
@@ -5568,7 +5569,7 @@
     </row>
     <row r="72" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q72" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44.5</v>
       </c>
       <c r="R72" s="3"/>
@@ -5579,7 +5580,7 @@
         <v>3</v>
       </c>
       <c r="U72" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V72" s="3" t="s">
@@ -5589,7 +5590,7 @@
         <v>1.5</v>
       </c>
       <c r="Y72" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>59</v>
       </c>
       <c r="AA72" t="s">
@@ -5599,7 +5600,7 @@
         <v>1</v>
       </c>
       <c r="AC72" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD72" t="s">
@@ -5611,7 +5612,7 @@
     </row>
     <row r="73" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q73" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="R73" s="3"/>
@@ -5622,7 +5623,7 @@
         <v>3</v>
       </c>
       <c r="U73" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V73" s="3" t="s">
@@ -5632,7 +5633,7 @@
         <v>1</v>
       </c>
       <c r="Y73" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>59.5</v>
       </c>
       <c r="AA73" t="s">
@@ -5642,7 +5643,7 @@
         <v>1</v>
       </c>
       <c r="AC73" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD73" t="s">
@@ -5654,7 +5655,7 @@
     </row>
     <row r="74" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q74" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>45.5</v>
       </c>
       <c r="R74" s="3"/>
@@ -5665,7 +5666,7 @@
         <v>3</v>
       </c>
       <c r="U74" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V74" s="3" t="s">
@@ -5675,7 +5676,7 @@
         <v>0.5</v>
       </c>
       <c r="Y74" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>60</v>
       </c>
       <c r="AA74" t="s">
@@ -5685,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="AC74" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD74" t="s">
@@ -5697,7 +5698,7 @@
     </row>
     <row r="75" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q75" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>46</v>
       </c>
       <c r="R75" s="6" t="s">
@@ -5710,7 +5711,7 @@
         <v>2</v>
       </c>
       <c r="U75" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V75" s="3" t="s">
@@ -5720,7 +5721,7 @@
         <v>4.5</v>
       </c>
       <c r="Y75" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>60.5</v>
       </c>
       <c r="Z75" t="s">
@@ -5733,7 +5734,7 @@
         <v>1</v>
       </c>
       <c r="AC75" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD75" t="s">
@@ -5745,7 +5746,7 @@
     </row>
     <row r="76" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q76" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>46.5</v>
       </c>
       <c r="R76" s="3"/>
@@ -5756,7 +5757,7 @@
         <v>2</v>
       </c>
       <c r="U76" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V76" s="3" t="s">
@@ -5766,7 +5767,7 @@
         <v>4</v>
       </c>
       <c r="Y76" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>61</v>
       </c>
       <c r="AA76" t="s">
@@ -5776,7 +5777,7 @@
         <v>1</v>
       </c>
       <c r="AC76" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD76" t="s">
@@ -5788,7 +5789,7 @@
     </row>
     <row r="77" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q77" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>47</v>
       </c>
       <c r="R77" s="3"/>
@@ -5799,7 +5800,7 @@
         <v>2</v>
       </c>
       <c r="U77" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V77" s="3" t="s">
@@ -5809,7 +5810,7 @@
         <v>3.5</v>
       </c>
       <c r="Y77" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>61.5</v>
       </c>
       <c r="AA77" t="s">
@@ -5819,7 +5820,7 @@
         <v>1</v>
       </c>
       <c r="AC77" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD77" t="s">
@@ -5831,7 +5832,7 @@
     </row>
     <row r="78" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q78" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>47.5</v>
       </c>
       <c r="R78" s="3"/>
@@ -5842,7 +5843,7 @@
         <v>2</v>
       </c>
       <c r="U78" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V78" s="3" t="s">
@@ -5852,7 +5853,7 @@
         <v>3</v>
       </c>
       <c r="Y78" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>62</v>
       </c>
       <c r="AA78" t="s">
@@ -5862,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="AC78" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD78" t="s">
@@ -5874,7 +5875,7 @@
     </row>
     <row r="79" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q79" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
       <c r="R79" s="3"/>
@@ -5885,7 +5886,7 @@
         <v>2</v>
       </c>
       <c r="U79" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V79" s="3" t="s">
@@ -5895,7 +5896,7 @@
         <v>2.5</v>
       </c>
       <c r="Y79" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>62.5</v>
       </c>
       <c r="AA79" t="s">
@@ -5905,7 +5906,7 @@
         <v>1</v>
       </c>
       <c r="AC79" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD79" t="s">
@@ -5917,7 +5918,7 @@
     </row>
     <row r="80" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q80" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>48.5</v>
       </c>
       <c r="R80" s="3"/>
@@ -5928,7 +5929,7 @@
         <v>2</v>
       </c>
       <c r="U80" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V80" s="3" t="s">
@@ -5938,7 +5939,7 @@
         <v>2</v>
       </c>
       <c r="Y80" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>63</v>
       </c>
       <c r="AA80" t="s">
@@ -5948,7 +5949,7 @@
         <v>1</v>
       </c>
       <c r="AC80" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD80" t="s">
@@ -5960,7 +5961,7 @@
     </row>
     <row r="81" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q81" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="R81" s="5" t="s">
@@ -5973,7 +5974,7 @@
         <v>3</v>
       </c>
       <c r="U81" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V81" s="3" t="s">
@@ -5983,7 +5984,7 @@
         <v>1.5</v>
       </c>
       <c r="Y81" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>63.5</v>
       </c>
       <c r="AA81" t="s">
@@ -5993,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="AC81" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD81" t="s">
@@ -6005,7 +6006,7 @@
     </row>
     <row r="82" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q82" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>49.5</v>
       </c>
       <c r="R82" s="3"/>
@@ -6016,7 +6017,7 @@
         <v>3</v>
       </c>
       <c r="U82" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V82" s="3" t="s">
@@ -6026,7 +6027,7 @@
         <v>1</v>
       </c>
       <c r="Y82" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="AA82" t="s">
@@ -6036,7 +6037,7 @@
         <v>1</v>
       </c>
       <c r="AC82" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD82" t="s">
@@ -6048,7 +6049,7 @@
     </row>
     <row r="83" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q83" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="R83" s="3"/>
@@ -6059,7 +6060,7 @@
         <v>3</v>
       </c>
       <c r="U83" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V83" s="3" t="s">
@@ -6069,7 +6070,7 @@
         <v>0.5</v>
       </c>
       <c r="Y83" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>64.5</v>
       </c>
       <c r="Z83" t="s">
@@ -6082,7 +6083,7 @@
         <v>2</v>
       </c>
       <c r="AC83" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD83" t="s">
@@ -6094,7 +6095,7 @@
     </row>
     <row r="84" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q84" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>50.5</v>
       </c>
       <c r="R84" s="3"/>
@@ -6105,7 +6106,7 @@
         <v>2</v>
       </c>
       <c r="U84" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V84" s="3" t="s">
@@ -6115,7 +6116,7 @@
         <v>4.5</v>
       </c>
       <c r="Y84" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>65</v>
       </c>
       <c r="AA84" t="s">
@@ -6125,7 +6126,7 @@
         <v>1</v>
       </c>
       <c r="AC84" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD84" t="s">
@@ -6137,7 +6138,7 @@
     </row>
     <row r="85" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q85" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>51</v>
       </c>
       <c r="R85" s="3"/>
@@ -6148,7 +6149,7 @@
         <v>2</v>
       </c>
       <c r="U85" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V85" s="3" t="s">
@@ -6158,7 +6159,7 @@
         <v>4</v>
       </c>
       <c r="Y85" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>65.5</v>
       </c>
       <c r="AA85" t="s">
@@ -6168,7 +6169,7 @@
         <v>1</v>
       </c>
       <c r="AC85" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD85" t="s">
@@ -6180,7 +6181,7 @@
     </row>
     <row r="86" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q86" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>51.5</v>
       </c>
       <c r="R86" s="3"/>
@@ -6191,7 +6192,7 @@
         <v>2</v>
       </c>
       <c r="U86" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.931640625</v>
       </c>
       <c r="V86" s="3" t="s">
@@ -6201,7 +6202,7 @@
         <v>3.5</v>
       </c>
       <c r="Y86" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>66</v>
       </c>
       <c r="AA86" t="s">
@@ -6211,7 +6212,7 @@
         <v>1</v>
       </c>
       <c r="AC86" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD86" t="s">
@@ -6223,7 +6224,7 @@
     </row>
     <row r="87" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q87" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>52</v>
       </c>
       <c r="R87" s="3" t="s">
@@ -6236,7 +6237,7 @@
         <v>3</v>
       </c>
       <c r="U87" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V87" s="3" t="s">
@@ -6246,7 +6247,7 @@
         <v>3</v>
       </c>
       <c r="Y87" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>66.5</v>
       </c>
       <c r="AA87" t="s">
@@ -6256,7 +6257,7 @@
         <v>1</v>
       </c>
       <c r="AC87" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD87" t="s">
@@ -6268,7 +6269,7 @@
     </row>
     <row r="88" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q88" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>52.5</v>
       </c>
       <c r="R88" s="3"/>
@@ -6279,7 +6280,7 @@
         <v>3</v>
       </c>
       <c r="U88" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V88" s="3" t="s">
@@ -6289,7 +6290,7 @@
         <v>2.5</v>
       </c>
       <c r="Y88" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>67</v>
       </c>
       <c r="AA88" t="s">
@@ -6299,7 +6300,7 @@
         <v>1</v>
       </c>
       <c r="AC88" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD88" t="s">
@@ -6311,7 +6312,7 @@
     </row>
     <row r="89" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q89" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>53</v>
       </c>
       <c r="R89" s="3"/>
@@ -6322,7 +6323,7 @@
         <v>3</v>
       </c>
       <c r="U89" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V89" s="3" t="s">
@@ -6332,7 +6333,7 @@
         <v>2</v>
       </c>
       <c r="Y89" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>67.5</v>
       </c>
       <c r="AA89" t="s">
@@ -6342,7 +6343,7 @@
         <v>1</v>
       </c>
       <c r="AC89" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD89" t="s">
@@ -6354,7 +6355,7 @@
     </row>
     <row r="90" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q90" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>53.5</v>
       </c>
       <c r="R90" s="3"/>
@@ -6365,7 +6366,7 @@
         <v>3</v>
       </c>
       <c r="U90" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V90" s="3" t="s">
@@ -6375,7 +6376,7 @@
         <v>1.5</v>
       </c>
       <c r="Y90" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>68</v>
       </c>
       <c r="AA90" t="s">
@@ -6385,7 +6386,7 @@
         <v>1</v>
       </c>
       <c r="AC90" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD90" t="s">
@@ -6397,7 +6398,7 @@
     </row>
     <row r="91" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q91" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>54</v>
       </c>
       <c r="R91" s="3"/>
@@ -6408,7 +6409,7 @@
         <v>3</v>
       </c>
       <c r="U91" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V91" s="3" t="s">
@@ -6418,7 +6419,7 @@
         <v>1</v>
       </c>
       <c r="Y91" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>68.5</v>
       </c>
       <c r="Z91" t="s">
@@ -6431,7 +6432,7 @@
         <v>2</v>
       </c>
       <c r="AC91" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD91" t="s">
@@ -6443,7 +6444,7 @@
     </row>
     <row r="92" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q92" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>54.5</v>
       </c>
       <c r="R92" s="3"/>
@@ -6454,7 +6455,7 @@
         <v>3</v>
       </c>
       <c r="U92" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V92" s="3" t="s">
@@ -6464,7 +6465,7 @@
         <v>0.5</v>
       </c>
       <c r="Y92" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>69</v>
       </c>
       <c r="AA92" t="s">
@@ -6474,7 +6475,7 @@
         <v>2</v>
       </c>
       <c r="AC92" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD92" t="s">
@@ -6486,7 +6487,7 @@
     </row>
     <row r="93" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q93" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>55</v>
       </c>
       <c r="R93" s="3" t="s">
@@ -6499,7 +6500,7 @@
         <v>3</v>
       </c>
       <c r="U93" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V93" s="3" t="s">
@@ -6509,7 +6510,7 @@
         <v>4.5</v>
       </c>
       <c r="Y93" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>69.5</v>
       </c>
       <c r="AA93" t="s">
@@ -6519,7 +6520,7 @@
         <v>1</v>
       </c>
       <c r="AC93" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD93" t="s">
@@ -6531,7 +6532,7 @@
     </row>
     <row r="94" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q94" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>55.5</v>
       </c>
       <c r="R94" s="3"/>
@@ -6542,7 +6543,7 @@
         <v>3</v>
       </c>
       <c r="U94" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V94" s="3" t="s">
@@ -6552,7 +6553,7 @@
         <v>4</v>
       </c>
       <c r="Y94" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>70</v>
       </c>
       <c r="AA94" t="s">
@@ -6562,7 +6563,7 @@
         <v>1</v>
       </c>
       <c r="AC94" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD94" t="s">
@@ -6574,7 +6575,7 @@
     </row>
     <row r="95" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q95" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>56</v>
       </c>
       <c r="R95" s="3"/>
@@ -6585,7 +6586,7 @@
         <v>3</v>
       </c>
       <c r="U95" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V95" s="3" t="s">
@@ -6595,7 +6596,7 @@
         <v>3.5</v>
       </c>
       <c r="Y95" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>70.5</v>
       </c>
       <c r="AA95" t="s">
@@ -6605,7 +6606,7 @@
         <v>1</v>
       </c>
       <c r="AC95" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD95" t="s">
@@ -6617,7 +6618,7 @@
     </row>
     <row r="96" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q96" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>56.5</v>
       </c>
       <c r="R96" s="3"/>
@@ -6628,7 +6629,7 @@
         <v>3</v>
       </c>
       <c r="U96" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V96" s="3" t="s">
@@ -6638,7 +6639,7 @@
         <v>3</v>
       </c>
       <c r="Y96" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>71</v>
       </c>
       <c r="AA96" t="s">
@@ -6648,7 +6649,7 @@
         <v>1</v>
       </c>
       <c r="AC96" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD96" t="s">
@@ -6660,7 +6661,7 @@
     </row>
     <row r="97" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q97" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>57</v>
       </c>
       <c r="R97" s="3"/>
@@ -6671,7 +6672,7 @@
         <v>3</v>
       </c>
       <c r="U97" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V97" s="3" t="s">
@@ -6681,7 +6682,7 @@
         <v>2.5</v>
       </c>
       <c r="Y97" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>71.5</v>
       </c>
       <c r="AA97" t="s">
@@ -6691,7 +6692,7 @@
         <v>1</v>
       </c>
       <c r="AC97" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD97" t="s">
@@ -6703,7 +6704,7 @@
     </row>
     <row r="98" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q98" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>57.5</v>
       </c>
       <c r="R98" s="3"/>
@@ -6714,7 +6715,7 @@
         <v>3</v>
       </c>
       <c r="U98" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>82.3974609375</v>
       </c>
       <c r="V98" s="3" t="s">
@@ -6724,7 +6725,7 @@
         <v>2</v>
       </c>
       <c r="Y98" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>72</v>
       </c>
       <c r="AA98" t="s">
@@ -6734,7 +6735,7 @@
         <v>1</v>
       </c>
       <c r="AC98" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD98" t="s">
@@ -6746,7 +6747,7 @@
     </row>
     <row r="99" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q99" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>58</v>
       </c>
       <c r="R99" s="5" t="s">
@@ -6759,7 +6760,7 @@
         <v>3</v>
       </c>
       <c r="U99" s="3">
-        <f>((1125 * T99)/(4 * 1024)) * 100</f>
+        <f t="shared" ref="U99:U105" si="16">((1125 * T99)/(4 * 1024)) * 100</f>
         <v>82.3974609375</v>
       </c>
       <c r="V99" s="3" t="s">
@@ -6769,7 +6770,7 @@
         <v>3</v>
       </c>
       <c r="Y99" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>72.5</v>
       </c>
       <c r="Z99" t="s">
@@ -6782,7 +6783,7 @@
         <v>2</v>
       </c>
       <c r="AC99" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD99" t="s">
@@ -6794,7 +6795,7 @@
     </row>
     <row r="100" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q100" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>58.5</v>
       </c>
       <c r="R100" s="3"/>
@@ -6805,7 +6806,7 @@
         <v>3</v>
       </c>
       <c r="U100" s="3">
-        <f>((1125 * T100)/(4 * 1024)) * 100</f>
+        <f t="shared" si="16"/>
         <v>82.3974609375</v>
       </c>
       <c r="V100" s="3" t="s">
@@ -6815,7 +6816,7 @@
         <v>2.5</v>
       </c>
       <c r="Y100" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>73</v>
       </c>
       <c r="AA100" t="s">
@@ -6825,7 +6826,7 @@
         <v>2</v>
       </c>
       <c r="AC100" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD100" t="s">
@@ -6837,7 +6838,7 @@
     </row>
     <row r="101" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q101" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="R101" s="3"/>
@@ -6848,7 +6849,7 @@
         <v>3</v>
       </c>
       <c r="U101" s="3">
-        <f>((1125 * T101)/(4 * 1024)) * 100</f>
+        <f t="shared" si="16"/>
         <v>82.3974609375</v>
       </c>
       <c r="V101" s="3" t="s">
@@ -6858,7 +6859,7 @@
         <v>2</v>
       </c>
       <c r="Y101" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>73.5</v>
       </c>
       <c r="AA101" t="s">
@@ -6868,7 +6869,7 @@
         <v>2</v>
       </c>
       <c r="AC101" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD101" t="s">
@@ -6880,7 +6881,7 @@
     </row>
     <row r="102" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q102" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>59.5</v>
       </c>
       <c r="R102" s="3"/>
@@ -6891,7 +6892,7 @@
         <v>3</v>
       </c>
       <c r="U102" s="3">
-        <f>((1125 * T102)/(4 * 1024)) * 100</f>
+        <f t="shared" si="16"/>
         <v>82.3974609375</v>
       </c>
       <c r="V102" s="3" t="s">
@@ -6901,7 +6902,7 @@
         <v>1.5</v>
       </c>
       <c r="Y102" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>74</v>
       </c>
       <c r="AA102" t="s">
@@ -6911,7 +6912,7 @@
         <v>1</v>
       </c>
       <c r="AC102" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD102" t="s">
@@ -6923,7 +6924,7 @@
     </row>
     <row r="103" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q103" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>60</v>
       </c>
       <c r="R103" s="3"/>
@@ -6934,7 +6935,7 @@
         <v>3</v>
       </c>
       <c r="U103" s="3">
-        <f>((1125 * T103)/(4 * 1024)) * 100</f>
+        <f t="shared" si="16"/>
         <v>82.3974609375</v>
       </c>
       <c r="V103" s="3" t="s">
@@ -6944,7 +6945,7 @@
         <v>1</v>
       </c>
       <c r="Y103" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>74.5</v>
       </c>
       <c r="AA103" t="s">
@@ -6954,7 +6955,7 @@
         <v>1</v>
       </c>
       <c r="AC103" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD103" t="s">
@@ -6966,7 +6967,7 @@
     </row>
     <row r="104" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q104" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>60.5</v>
       </c>
       <c r="R104" s="3"/>
@@ -6977,7 +6978,7 @@
         <v>3</v>
       </c>
       <c r="U104" s="3">
-        <f>((1125 * T104)/(4 * 1024)) * 100</f>
+        <f t="shared" si="16"/>
         <v>82.3974609375</v>
       </c>
       <c r="V104" s="3" t="s">
@@ -6987,7 +6988,7 @@
         <v>0.5</v>
       </c>
       <c r="Y104" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>75</v>
       </c>
       <c r="AA104" t="s">
@@ -6997,7 +6998,7 @@
         <v>1</v>
       </c>
       <c r="AC104" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD104" t="s">
@@ -7009,7 +7010,7 @@
     </row>
     <row r="105" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Q105" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>61</v>
       </c>
       <c r="R105" s="3" t="s">
@@ -7022,7 +7023,7 @@
         <v>3</v>
       </c>
       <c r="U105" s="3">
-        <f>((1125 * T105)/(4 * 1024)) * 100</f>
+        <f t="shared" si="16"/>
         <v>82.3974609375</v>
       </c>
       <c r="V105" s="3" t="s">
@@ -7032,7 +7033,7 @@
         <v>4.5</v>
       </c>
       <c r="Y105" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>75.5</v>
       </c>
       <c r="AA105" t="s">
@@ -7042,7 +7043,7 @@
         <v>1</v>
       </c>
       <c r="AC105" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD105" t="s">
@@ -7054,7 +7055,7 @@
     </row>
     <row r="106" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y106" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="AA106" t="s">
@@ -7064,7 +7065,7 @@
         <v>1</v>
       </c>
       <c r="AC106" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD106" t="s">
@@ -7076,7 +7077,7 @@
     </row>
     <row r="107" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y107" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>76.5</v>
       </c>
       <c r="Z107" t="s">
@@ -7089,7 +7090,7 @@
         <v>2</v>
       </c>
       <c r="AC107" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD107" t="s">
@@ -7101,7 +7102,7 @@
     </row>
     <row r="108" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y108" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>77</v>
       </c>
       <c r="AA108" t="s">
@@ -7111,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="AC108" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD108" t="s">
@@ -7123,7 +7124,7 @@
     </row>
     <row r="109" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y109" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>77.5</v>
       </c>
       <c r="AA109" t="s">
@@ -7133,7 +7134,7 @@
         <v>2</v>
       </c>
       <c r="AC109" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD109" t="s">
@@ -7145,7 +7146,7 @@
     </row>
     <row r="110" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y110" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>78</v>
       </c>
       <c r="AA110" t="s">
@@ -7155,7 +7156,7 @@
         <v>2</v>
       </c>
       <c r="AC110" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD110" t="s">
@@ -7167,7 +7168,7 @@
     </row>
     <row r="111" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y111" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>78.5</v>
       </c>
       <c r="AA111" t="s">
@@ -7177,7 +7178,7 @@
         <v>1</v>
       </c>
       <c r="AC111" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD111" t="s">
@@ -7189,7 +7190,7 @@
     </row>
     <row r="112" spans="17:31" x14ac:dyDescent="0.25">
       <c r="Y112" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>79</v>
       </c>
       <c r="AA112" t="s">
@@ -7199,7 +7200,7 @@
         <v>1</v>
       </c>
       <c r="AC112" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD112" t="s">
@@ -7211,7 +7212,7 @@
     </row>
     <row r="113" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y113" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>79.5</v>
       </c>
       <c r="AA113" t="s">
@@ -7221,7 +7222,7 @@
         <v>1</v>
       </c>
       <c r="AC113" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD113" t="s">
@@ -7233,7 +7234,7 @@
     </row>
     <row r="114" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y114" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>80</v>
       </c>
       <c r="AA114" t="s">
@@ -7243,7 +7244,7 @@
         <v>1</v>
       </c>
       <c r="AC114" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.62109375</v>
       </c>
       <c r="AD114" t="s">
@@ -7255,7 +7256,7 @@
     </row>
     <row r="115" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y115" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>80.5</v>
       </c>
       <c r="Z115" t="s">
@@ -7268,7 +7269,7 @@
         <v>2</v>
       </c>
       <c r="AC115" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73.2421875</v>
       </c>
       <c r="AD115" t="s">

</xml_diff>